<commit_message>
Update control flux log
</commit_message>
<xml_diff>
--- a/commissioning_information/control_flux_files_counts.xlsx
+++ b/commissioning_information/control_flux_files_counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\data\proposal\00113\Control_flux_measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0008A9-99DC-4538-B529-B3EA1AA3C053}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62ECA6B-E7CE-4D8C-9EA2-6619BEB430E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7875" yWindow="75" windowWidth="27060" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="138">
   <si>
     <t>BBY0010699.tar</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Time to correct the equation!!!</t>
   </si>
   <si>
-    <t>Add pi to the area &amp; get all units in m</t>
-  </si>
-  <si>
     <t>Sapmot, cm</t>
   </si>
   <si>
@@ -359,6 +356,84 @@
   </si>
   <si>
     <t>vs 17.7% resolution above</t>
+  </si>
+  <si>
+    <t>back to 17.7% resolution above</t>
+  </si>
+  <si>
+    <t>BBY0054487.tar</t>
+  </si>
+  <si>
+    <t>BBY0054488.tar</t>
+  </si>
+  <si>
+    <t>BBY0054489.tar</t>
+  </si>
+  <si>
+    <t>BBY0054490.tar</t>
+  </si>
+  <si>
+    <t>BBY0054491.tar</t>
+  </si>
+  <si>
+    <t>BBY0054492.tar</t>
+  </si>
+  <si>
+    <t>BBY0054493.tar</t>
+  </si>
+  <si>
+    <t>This set is wrong because I forgot to insert guard aperture</t>
+  </si>
+  <si>
+    <t>BBY0054496.tar</t>
+  </si>
+  <si>
+    <t>BBY0054497.tar</t>
+  </si>
+  <si>
+    <t>BBY0054498.tar</t>
+  </si>
+  <si>
+    <t>BBY0054499.tar</t>
+  </si>
+  <si>
+    <t>BBY0054500.tar</t>
+  </si>
+  <si>
+    <t>BBY0054501.tar</t>
+  </si>
+  <si>
+    <t>not much luck something was wrong with choppers from here</t>
+  </si>
+  <si>
+    <t>1 guide</t>
+  </si>
+  <si>
+    <t>2 guides</t>
+  </si>
+  <si>
+    <t>4 guides</t>
+  </si>
+  <si>
+    <t>5 guides</t>
+  </si>
+  <si>
+    <t>Add pi to the area &amp; get all units in cm</t>
+  </si>
+  <si>
+    <t>3 guides - reflections</t>
+  </si>
+  <si>
+    <t>Three first guides are very repeatable</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>spectra_extraction.py</t>
+  </si>
+  <si>
+    <t>in P113</t>
   </si>
 </sst>
 </file>
@@ -371,7 +446,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +633,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC69720"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -905,7 +988,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -940,11 +1023,22 @@
     <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="15" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1240,7 +1334,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>399</xdr:rowOff>
     </xdr:to>
@@ -1372,7 +1466,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>994581</xdr:colOff>
+      <xdr:colOff>1032681</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>119903</xdr:rowOff>
     </xdr:to>
@@ -1529,6 +1623,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>61635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>18382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC34614A-334E-4CC6-83CB-51CB2B184D47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="47848560"/>
+          <a:ext cx="5324475" cy="3766747"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1855,16 +1993,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O223"/>
+  <dimension ref="A1:O248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I214" sqref="I214"/>
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F248" sqref="F248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -2528,12 +2666,12 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -4378,7 +4516,7 @@
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B173" t="s">
         <v>3</v>
@@ -4409,7 +4547,7 @@
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B174" t="s">
         <v>4</v>
@@ -4440,7 +4578,7 @@
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
@@ -4519,7 +4657,7 @@
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B182" t="s">
         <v>3</v>
@@ -4550,7 +4688,7 @@
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B183" t="s">
         <v>4</v>
@@ -4581,7 +4719,7 @@
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B184" t="s">
         <v>5</v>
@@ -4662,7 +4800,7 @@
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B190" t="s">
         <v>3</v>
@@ -4693,7 +4831,7 @@
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B191" t="s">
         <v>4</v>
@@ -4724,7 +4862,7 @@
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B192" t="s">
         <v>5</v>
@@ -4769,22 +4907,22 @@
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A197" s="20">
+      <c r="A197" s="18">
         <v>44603</v>
       </c>
-      <c r="B197" s="21"/>
+      <c r="B197" s="19"/>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A198" s="21" t="s">
+      <c r="A198" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B198" s="21"/>
+      <c r="B198" s="19"/>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A199" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B199" s="21"/>
+      <c r="A199" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B199" s="19"/>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
@@ -4795,30 +4933,30 @@
       </c>
       <c r="C201" s="9"/>
       <c r="D201" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F201" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G201" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G201" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H201" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I201" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J201" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="J201" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B202" t="s">
         <v>3</v>
@@ -4854,7 +4992,7 @@
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B203" t="s">
         <v>4</v>
@@ -4876,7 +5014,7 @@
         <f>D203/((PI()*(F203/2)^2))*G203^2</f>
         <v>1016136333794.3768</v>
       </c>
-      <c r="I203" s="22">
+      <c r="I203" s="20">
         <f>H203/(PI()*2^2)</f>
         <v>80861560189.325607</v>
       </c>
@@ -4890,7 +5028,7 @@
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B204" t="s">
         <v>5</v>
@@ -4927,10 +5065,10 @@
     </row>
     <row r="206" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C206" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C206" s="11" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="208" spans="1:15" x14ac:dyDescent="0.25">
@@ -4942,30 +5080,30 @@
       </c>
       <c r="C208" s="9"/>
       <c r="D208" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E208" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F208" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G208" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G208" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H208" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I208" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J208" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="J208" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B209" t="s">
         <v>3</v>
@@ -4997,7 +5135,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B210" t="s">
         <v>4</v>
@@ -5018,7 +5156,7 @@
         <f t="shared" ref="H210:H218" si="13">D210/((PI()*(F210/2)^2))*G210^2</f>
         <v>537587581256.31201</v>
       </c>
-      <c r="I210" s="22">
+      <c r="I210" s="20">
         <f t="shared" ref="I210:I218" si="14">H210/(PI()*2^2)</f>
         <v>42779860450.878998</v>
       </c>
@@ -5029,7 +5167,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B211" t="s">
         <v>5</v>
@@ -5090,30 +5228,30 @@
       </c>
       <c r="C215" s="9"/>
       <c r="D215" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E215" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F215" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G215" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G215" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I215" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J215" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="J215" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B216" t="s">
         <v>3</v>
@@ -5145,7 +5283,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B217" t="s">
         <v>4</v>
@@ -5166,7 +5304,7 @@
         <f t="shared" si="13"/>
         <v>543516790633.0387</v>
       </c>
-      <c r="I217" s="22">
+      <c r="I217" s="20">
         <f t="shared" si="14"/>
         <v>43251691941.345436</v>
       </c>
@@ -5177,7 +5315,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B218" t="s">
         <v>5</v>
@@ -5217,14 +5355,502 @@
         <v>136</v>
       </c>
     </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B222" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H223" s="1"/>
-      <c r="I223" s="1"/>
-      <c r="J223" s="1"/>
+      <c r="A223" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C223" s="9"/>
+      <c r="D223" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E223" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H223" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I223" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J223" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B224" s="29"/>
+      <c r="C224" s="29"/>
+      <c r="D224" s="1"/>
+      <c r="E224" s="6"/>
+      <c r="F224" s="1"/>
+      <c r="G224" s="1"/>
+      <c r="H224" s="1"/>
+      <c r="I224" s="1"/>
+      <c r="J224" s="1"/>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>113</v>
+      </c>
+      <c r="B225" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225">
+        <v>315782</v>
+      </c>
+      <c r="D225">
+        <v>55127.633999999998</v>
+      </c>
+      <c r="F225">
+        <v>0.5</v>
+      </c>
+      <c r="G225">
+        <v>1677.6</v>
+      </c>
+      <c r="H225" s="16">
+        <f t="shared" ref="H225:H231" si="16">D225/((PI()*(F225/2)^2))*G225^2</f>
+        <v>790162288259.30493</v>
+      </c>
+      <c r="I225" s="16">
+        <f t="shared" ref="I225:I231" si="17">H225/(PI()*2^2)</f>
+        <v>62879117010.635742</v>
+      </c>
+      <c r="J225" s="17">
+        <f t="shared" ref="J225:J231" si="18">D225/(PI()*(F225/2)^2)</f>
+        <v>280762.73446594668</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>114</v>
+      </c>
+      <c r="B226" t="s">
+        <v>128</v>
+      </c>
+      <c r="C226">
+        <v>376488</v>
+      </c>
+      <c r="D226">
+        <v>65766.759000000005</v>
+      </c>
+      <c r="F226">
+        <v>0.5</v>
+      </c>
+      <c r="G226">
+        <v>1477.6</v>
+      </c>
+      <c r="H226" s="16">
+        <f t="shared" si="16"/>
+        <v>731291145642.94299</v>
+      </c>
+      <c r="I226" s="21">
+        <f t="shared" si="17"/>
+        <v>58194300334.204773</v>
+      </c>
+      <c r="J226" s="17">
+        <f t="shared" si="18"/>
+        <v>334947.35315146868</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>115</v>
+      </c>
+      <c r="B227" t="s">
+        <v>129</v>
+      </c>
+      <c r="C227">
+        <v>631838</v>
+      </c>
+      <c r="D227">
+        <v>110303.102</v>
+      </c>
+      <c r="F227">
+        <v>0.5</v>
+      </c>
+      <c r="G227">
+        <v>1277.5999999999999</v>
+      </c>
+      <c r="H227" s="16">
+        <f t="shared" si="16"/>
+        <v>916954196201.08813</v>
+      </c>
+      <c r="I227" s="16">
+        <f t="shared" si="17"/>
+        <v>72968896457.12941</v>
+      </c>
+      <c r="J227" s="17">
+        <f t="shared" si="18"/>
+        <v>561769.08549342491</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B228" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C228" s="22">
+        <v>269961</v>
+      </c>
+      <c r="D228" s="22">
+        <v>47128.434999999998</v>
+      </c>
+      <c r="E228" s="22"/>
+      <c r="F228" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="G228" s="22">
+        <v>1077.5999999999999</v>
+      </c>
+      <c r="H228" s="23">
+        <f t="shared" si="16"/>
+        <v>1114880411739.4175</v>
+      </c>
+      <c r="I228" s="23">
+        <f t="shared" si="17"/>
+        <v>88719364242.327911</v>
+      </c>
+      <c r="J228" s="24">
+        <f t="shared" si="18"/>
+        <v>960092.59397569136</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B229" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C229" s="22">
+        <v>1118159</v>
+      </c>
+      <c r="D229" s="22">
+        <v>195202.57800000001</v>
+      </c>
+      <c r="E229" s="22"/>
+      <c r="F229" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="G229" s="22">
+        <v>877.6</v>
+      </c>
+      <c r="H229" s="23">
+        <f t="shared" si="16"/>
+        <v>3062731176864.1855</v>
+      </c>
+      <c r="I229" s="23">
+        <f t="shared" si="17"/>
+        <v>243724403079.79654</v>
+      </c>
+      <c r="J229" s="24">
+        <f t="shared" si="18"/>
+        <v>3976634.2647016016</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B230" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C230" s="22">
+        <v>7803921</v>
+      </c>
+      <c r="D230" s="22">
+        <v>1362797.9920000001</v>
+      </c>
+      <c r="E230" s="22"/>
+      <c r="F230" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="G230" s="22">
+        <v>677.6</v>
+      </c>
+      <c r="H230" s="23">
+        <f t="shared" si="16"/>
+        <v>12747011597065.904</v>
+      </c>
+      <c r="I230" s="23">
+        <f t="shared" si="17"/>
+        <v>1014374952661.377</v>
+      </c>
+      <c r="J230" s="24">
+        <f t="shared" si="18"/>
+        <v>27762692.718401186</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B231" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C231" s="22">
+        <v>58761987</v>
+      </c>
+      <c r="D231" s="22">
+        <v>10277770.465</v>
+      </c>
+      <c r="E231" s="22"/>
+      <c r="F231" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="G231" s="22">
+        <v>476.4</v>
+      </c>
+      <c r="H231" s="23">
+        <f t="shared" si="16"/>
+        <v>47519572090137.945</v>
+      </c>
+      <c r="I231" s="23">
+        <f t="shared" si="17"/>
+        <v>3781487395878.5615</v>
+      </c>
+      <c r="J231" s="24">
+        <f t="shared" si="18"/>
+        <v>209377020.60398564</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B232" s="13">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B233" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C235" s="9"/>
+      <c r="D235" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E235" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H235" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I235" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J235" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>121</v>
+      </c>
+      <c r="B236" t="s">
+        <v>3</v>
+      </c>
+      <c r="C236">
+        <v>313275</v>
+      </c>
+      <c r="D236">
+        <v>54689.974999999999</v>
+      </c>
+      <c r="F236">
+        <v>0.5</v>
+      </c>
+      <c r="G236">
+        <v>1677.6</v>
+      </c>
+      <c r="H236" s="16">
+        <f>D236/((PI()*(F236/2)^2))*G236^2</f>
+        <v>783889179623.49316</v>
+      </c>
+      <c r="I236" s="16">
+        <f t="shared" ref="I236:I237" si="19">H236/(PI()*2^2)</f>
+        <v>62379918886.664787</v>
+      </c>
+      <c r="J236" s="25">
+        <f t="shared" ref="J236:J238" si="20">D236/(PI()*(F236/2)^2)</f>
+        <v>278533.75548230973</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>122</v>
+      </c>
+      <c r="B237" t="s">
+        <v>128</v>
+      </c>
+      <c r="C237">
+        <v>374452</v>
+      </c>
+      <c r="D237">
+        <v>65369.947999999997</v>
+      </c>
+      <c r="F237">
+        <v>0.5</v>
+      </c>
+      <c r="G237">
+        <v>1477.6</v>
+      </c>
+      <c r="H237" s="16">
+        <f t="shared" ref="H237:H238" si="21">D237/((PI()*(F237/2)^2))*G237^2</f>
+        <v>726878819793.13599</v>
+      </c>
+      <c r="I237" s="21">
+        <f t="shared" si="19"/>
+        <v>57843178599.4403</v>
+      </c>
+      <c r="J237" s="25">
+        <f t="shared" si="20"/>
+        <v>332926.41132352501</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>123</v>
+      </c>
+      <c r="B238" t="s">
+        <v>129</v>
+      </c>
+      <c r="C238">
+        <v>633809</v>
+      </c>
+      <c r="D238">
+        <v>110647.19</v>
+      </c>
+      <c r="F238">
+        <v>0.5</v>
+      </c>
+      <c r="G238">
+        <v>1277.5999999999999</v>
+      </c>
+      <c r="H238" s="16">
+        <f t="shared" si="21"/>
+        <v>919814613811.66846</v>
+      </c>
+      <c r="I238" s="16">
+        <f>H238/(PI()*2^2)</f>
+        <v>73196521258.144897</v>
+      </c>
+      <c r="J238" s="25">
+        <f t="shared" si="20"/>
+        <v>563521.51128730027</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>124</v>
+      </c>
+      <c r="B239" t="s">
+        <v>4</v>
+      </c>
+      <c r="C239">
+        <v>89649</v>
+      </c>
+      <c r="D239">
+        <v>15650.472</v>
+      </c>
+      <c r="E239" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>125</v>
+      </c>
+      <c r="B240" t="s">
+        <v>130</v>
+      </c>
+      <c r="C240">
+        <v>89442</v>
+      </c>
+      <c r="D240">
+        <v>15614.334999999999</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>126</v>
+      </c>
+      <c r="B241" t="s">
+        <v>131</v>
+      </c>
+      <c r="C241">
+        <v>816529</v>
+      </c>
+      <c r="D241">
+        <v>32780.966</v>
+      </c>
+      <c r="I241" s="17"/>
+      <c r="J241" s="17"/>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B242" s="13">
+        <v>44797</v>
+      </c>
+      <c r="H242" t="s">
+        <v>134</v>
+      </c>
+      <c r="I242" s="17"/>
+      <c r="J242" s="17"/>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B243" s="7">
+        <v>140</v>
+      </c>
+      <c r="I243" s="17"/>
+      <c r="J243" s="17"/>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F246" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F247" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F248" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A224:C224"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>